<commit_message>
New units, classifications items, regions added.
</commit_message>
<xml_diff>
--- a/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_2018_Sep_30.xlsx
+++ b/IEDC_content_fill/IEDC_Prototype_Datasets_Batch1_Upload_2018_Sep_30.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\Freiburg Implementation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\Software\IEDC_content_fill\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9396" tabRatio="477" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="477" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="13" r:id="rId1"/>
@@ -4738,11 +4738,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5510,8 +5510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="BF36" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="BF6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="BR54" sqref="BR54"/>

</xml_diff>